<commit_message>
incluido respostas das provas do modulo 4 da pos ead de adm e financas
</commit_message>
<xml_diff>
--- a/PosEAD  Adm e Finanças/Modulo 4/Provas/Gabarito das Provas.xlsx
+++ b/PosEAD  Adm e Finanças/Modulo 4/Provas/Gabarito das Provas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
   <si>
     <t>Conferido</t>
   </si>
@@ -36,6 +36,18 @@
   </si>
   <si>
     <t>Prova Mercado Financeiro nacional e internacional</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -426,7 +438,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,16 +493,36 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="L4" s="5" t="s">
         <v>0</v>
       </c>
@@ -542,16 +574,36 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="L10" s="5" t="s">
         <v>0</v>
       </c>
@@ -603,16 +655,36 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="L16" s="5" t="s">
         <v>0</v>
       </c>

</xml_diff>